<commit_message>
Detected if line is a label is done in ExecTimer not in each language Doc/Test code through variables
</commit_message>
<xml_diff>
--- a/DocSource/Complete Statement List.xlsx
+++ b/DocSource/Complete Statement List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nedlecky\GitHub\LEonard\DocSource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4B4BC0-6928-4E10-BB23-E103E685AFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A1C029-4E24-4239-91D5-2922C95DEF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44460" yWindow="720" windowWidth="30420" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="346">
   <si>
     <t>Statement</t>
   </si>
@@ -80,21 +80,12 @@
     <t>exec_lescript(filename)</t>
   </si>
   <si>
-    <t>illegal</t>
-  </si>
-  <si>
     <t>WHERE IS EXEC LINE for all 3 languages</t>
   </si>
   <si>
     <t>Variable Management</t>
   </si>
   <si>
-    <t>import_variables(filename)</t>
-  </si>
-  <si>
-    <t>system_variable(var_name, True|False)</t>
-  </si>
-  <si>
     <t>system_position(pos_name, True|False)</t>
   </si>
   <si>
@@ -164,19 +155,10 @@
     <t>pause</t>
   </si>
   <si>
-    <t>clear()</t>
-  </si>
-  <si>
-    <t>clear</t>
-  </si>
-  <si>
     <t>sleep(seconds)</t>
   </si>
   <si>
     <t>random(n, low, high)</t>
-  </si>
-  <si>
-    <t>assert(var_name, value</t>
   </si>
   <si>
     <t>jump(string label)</t>
@@ -1012,10 +994,79 @@
     <t>Python Library</t>
   </si>
   <si>
-    <t>system_variable: le_language</t>
-  </si>
-  <si>
     <t>Handled</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>using_languages</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>JavaPrint1.js
+JavaPrint2.js</t>
+  </si>
+  <si>
+    <t>exec_java</t>
+  </si>
+  <si>
+    <t>exec_python</t>
+  </si>
+  <si>
+    <t>PythonPrint1.js
+PythonPrint2.js</t>
+  </si>
+  <si>
+    <t>le_language (system variable)</t>
+  </si>
+  <si>
+    <t>le_read_var(string var_name)</t>
+  </si>
+  <si>
+    <t>le_write_var(string var_name, string value)</t>
+  </si>
+  <si>
+    <t>le_write_sysvar(string var_name, string value)</t>
+  </si>
+  <si>
+    <t>le_clear_variables()</t>
+  </si>
+  <si>
+    <t>le_import_variables(filename)</t>
+  </si>
+  <si>
+    <t>le_system_variable(var_name, True|False)</t>
+  </si>
+  <si>
+    <t>le_clear_variables</t>
+  </si>
+  <si>
+    <t>le_import_variables</t>
+  </si>
+  <si>
+    <t>Also Uses</t>
+  </si>
+  <si>
+    <t>import_test_data.txt</t>
+  </si>
+  <si>
+    <t>assert(var_name, value)</t>
+  </si>
+  <si>
+    <t>assert(bool condition)</t>
+  </si>
+  <si>
+    <t>Tested by
+LEScript</t>
+  </si>
+  <si>
+    <t>assert</t>
+  </si>
+  <si>
+    <t>variables</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1190,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1188,6 +1239,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1197,10 +1255,24 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFill="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Code" xfId="3" xr:uid="{FFE2B8D9-002C-49B1-A898-24176D5D7997}"/>
@@ -1422,16 +1494,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD1012"/>
+  <dimension ref="A1:AF1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.85546875" customWidth="1"/>
+    <col min="1" max="1" width="61.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" customWidth="1"/>
@@ -1439,30 +1511,36 @@
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.140625" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="42.42578125" customWidth="1"/>
+    <col min="9" max="9" width="27.85546875" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" customWidth="1"/>
+    <col min="11" max="11" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="18" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:11" s="18" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="J1" s="29"/>
+      <c r="K1" s="25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="18" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
+    <row r="2" spans="1:11" s="18" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25"/>
       <c r="B2" s="19" t="s">
         <v>4</v>
       </c>
@@ -1484,9 +1562,15 @@
       <c r="H2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="22"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="22" t="s">
+        <v>343</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>339</v>
+      </c>
+      <c r="K2" s="25"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -1494,7 +1578,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>12</v>
       </c>
@@ -1510,8 +1594,12 @@
       <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="J4" s="15"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>13</v>
       </c>
@@ -1527,8 +1615,12 @@
       <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="J5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>14</v>
       </c>
@@ -1544,10 +1636,14 @@
       <c r="E6" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I6" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>11</v>
@@ -1561,168 +1657,302 @@
       <c r="E7" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>327</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>328</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
         <v>18</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
-        <v>19</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4"/>
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="4"/>
+      <c r="E14" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="4"/>
+      <c r="E15" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="E16" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="30" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="30" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="30" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="30" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="30" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="30" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="30" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>11</v>
@@ -1730,9 +1960,9 @@
       <c r="C26" s="4"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>11</v>
@@ -1740,9 +1970,9 @@
       <c r="C27" s="4"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>11</v>
@@ -1750,33 +1980,35 @@
       <c r="C28" s="4"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15"/>
       <c r="B29" s="3"/>
       <c r="C29" s="4"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="4"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D31" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>11</v>
@@ -1784,117 +2016,157 @@
       <c r="C32" s="4"/>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="4"/>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D33" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="4"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D34" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C36" s="4"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="15"/>
-      <c r="B37" s="3"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:32" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C37" s="4"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" ht="15" x14ac:dyDescent="0.2">
+      <c r="A38" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C38" s="4"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="4"/>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:32" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="3" t="s">
+      <c r="D40" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="9"/>
+      <c r="S40" s="9"/>
+      <c r="T40" s="9"/>
+      <c r="U40" s="9"/>
+      <c r="V40" s="9"/>
+      <c r="W40" s="9"/>
+      <c r="X40" s="9"/>
+      <c r="Y40" s="9"/>
+      <c r="Z40" s="9"/>
+      <c r="AA40" s="9"/>
+      <c r="AB40" s="9"/>
+      <c r="AC40" s="9"/>
+      <c r="AD40" s="9"/>
+      <c r="AE40" s="9"/>
+      <c r="AF40" s="9"/>
+    </row>
+    <row r="41" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C41" s="4"/>
-      <c r="D41" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="4"/>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:32" ht="15" x14ac:dyDescent="0.2">
+      <c r="A43" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="3" t="s">
+      <c r="D43" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>11</v>
@@ -1902,9 +2174,9 @@
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>11</v>
@@ -1912,99 +2184,67 @@
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="I46" s="33" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="47" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A48" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="I47" s="33" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="48" spans="1:32" ht="15" x14ac:dyDescent="0.2">
+      <c r="A48" s="15"/>
+      <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="1:30" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>11</v>
-      </c>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A49" s="15"/>
+      <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:30" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>11</v>
-      </c>
+    <row r="50" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
-      <c r="J51" s="9"/>
-      <c r="K51" s="9"/>
-      <c r="L51" s="9"/>
-      <c r="M51" s="9"/>
-      <c r="N51" s="9"/>
-      <c r="O51" s="9"/>
-      <c r="P51" s="9"/>
-      <c r="Q51" s="9"/>
-      <c r="R51" s="9"/>
-      <c r="S51" s="9"/>
-      <c r="T51" s="9"/>
-      <c r="U51" s="9"/>
-      <c r="V51" s="9"/>
-      <c r="W51" s="9"/>
-      <c r="X51" s="9"/>
-      <c r="Y51" s="9"/>
-      <c r="Z51" s="9"/>
-      <c r="AA51" s="9"/>
-      <c r="AB51" s="9"/>
-      <c r="AC51" s="9"/>
-      <c r="AD51" s="9"/>
-    </row>
-    <row r="52" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>11</v>
@@ -2012,9 +2252,9 @@
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>11</v>
@@ -2022,115 +2262,111 @@
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D54" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" spans="1:30" ht="15" x14ac:dyDescent="0.2">
-      <c r="A55" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+    </row>
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A55" s="15"/>
+      <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:30" ht="15" x14ac:dyDescent="0.2">
-      <c r="A56" s="15" t="s">
+    <row r="56" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:30" ht="15" x14ac:dyDescent="0.2">
-      <c r="A57" s="15"/>
-      <c r="B57" s="4"/>
+    <row r="57" spans="1:4" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:30" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
-        <v>58</v>
-      </c>
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="1:30" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>11</v>
-      </c>
+    <row r="59" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" s="3"/>
       <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-    </row>
-    <row r="60" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-    </row>
-    <row r="61" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="15" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-    </row>
-    <row r="62" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-    </row>
-    <row r="63" spans="1:30" ht="15" x14ac:dyDescent="0.2">
-      <c r="A63" s="15"/>
-      <c r="B63" s="4"/>
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-    </row>
-    <row r="64" spans="1:30" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B64" s="4"/>
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-    </row>
-    <row r="65" spans="1:4" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D64" s="3"/>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B65" s="3"/>
       <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
+      <c r="D65" s="3"/>
     </row>
     <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
@@ -7766,60 +8002,13 @@
       <c r="C1004" s="4"/>
       <c r="D1004" s="4"/>
     </row>
-    <row r="1005" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1005" s="5"/>
-      <c r="B1005" s="4"/>
-      <c r="C1005" s="4"/>
-      <c r="D1005" s="4"/>
-    </row>
-    <row r="1006" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1006" s="5"/>
-      <c r="B1006" s="4"/>
-      <c r="C1006" s="4"/>
-      <c r="D1006" s="4"/>
-    </row>
-    <row r="1007" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1007" s="5"/>
-      <c r="B1007" s="4"/>
-      <c r="C1007" s="4"/>
-      <c r="D1007" s="4"/>
-    </row>
-    <row r="1008" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1008" s="5"/>
-      <c r="B1008" s="4"/>
-      <c r="C1008" s="4"/>
-      <c r="D1008" s="4"/>
-    </row>
-    <row r="1009" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1009" s="5"/>
-      <c r="B1009" s="4"/>
-      <c r="C1009" s="4"/>
-      <c r="D1009" s="4"/>
-    </row>
-    <row r="1010" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1010" s="5"/>
-      <c r="B1010" s="4"/>
-      <c r="C1010" s="4"/>
-      <c r="D1010" s="4"/>
-    </row>
-    <row r="1011" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1011" s="5"/>
-      <c r="B1011" s="4"/>
-      <c r="C1011" s="4"/>
-      <c r="D1011" s="4"/>
-    </row>
-    <row r="1012" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1012" s="5"/>
-      <c r="B1012" s="4"/>
-      <c r="C1012" s="4"/>
-      <c r="D1012" s="4"/>
-    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7831,11 +8020,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AE1075"/>
+  <dimension ref="A1:AE1076"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7853,24 +8042,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>325</v>
-      </c>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22" t="s">
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="1"/>
@@ -7896,8 +8085,8 @@
       <c r="AE1" s="1"/>
     </row>
     <row r="2" spans="1:31" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="24"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="19" t="s">
         <v>4</v>
       </c>
@@ -7919,7 +8108,7 @@
       <c r="I2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="22"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -7944,7 +8133,7 @@
     </row>
     <row r="3" spans="1:31" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
@@ -7957,7 +8146,7 @@
     </row>
     <row r="4" spans="1:31" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
@@ -7982,7 +8171,7 @@
     </row>
     <row r="6" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="11"/>
@@ -7995,13 +8184,13 @@
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
@@ -8012,13 +8201,13 @@
     </row>
     <row r="8" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B8" s="10">
         <v>98</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
@@ -8029,13 +8218,13 @@
     </row>
     <row r="9" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B9" s="10">
         <v>99</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -8056,7 +8245,7 @@
     </row>
     <row r="11" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
@@ -8069,7 +8258,7 @@
     </row>
     <row r="12" spans="1:31" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="11" t="s">
@@ -8084,22 +8273,15 @@
     </row>
     <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+        <v>20</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="11" t="s">
@@ -8114,7 +8296,7 @@
     </row>
     <row r="15" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="11" t="s">
@@ -8122,17 +8304,14 @@
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="14" t="s">
-        <v>78</v>
-      </c>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="11" t="s">
@@ -8140,14 +8319,17 @@
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="14" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="11" t="s">
@@ -8162,7 +8344,7 @@
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="11" t="s">
@@ -8177,7 +8359,7 @@
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="11" t="s">
@@ -8192,13 +8374,11 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>84</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B20" s="10"/>
       <c r="C20" s="11" t="s">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
@@ -8208,8 +8388,15 @@
       <c r="I20" s="12"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
+      <c r="A21" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -8217,10 +8404,7 @@
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
     </row>
-    <row r="22" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>85</v>
-      </c>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="D22" s="12"/>
@@ -8230,16 +8414,12 @@
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>70</v>
-      </c>
+    <row r="23" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
@@ -8247,15 +8427,15 @@
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
@@ -8266,13 +8446,13 @@
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
@@ -8282,8 +8462,15 @@
       <c r="I25" s="12"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="10"/>
-      <c r="C26" s="11"/>
+      <c r="A26" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
@@ -8292,15 +8479,8 @@
       <c r="I26" s="12"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="11"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
@@ -8310,13 +8490,13 @@
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
@@ -8327,13 +8507,13 @@
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
@@ -8343,8 +8523,15 @@
       <c r="I29" s="12"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="10"/>
-      <c r="C30" s="11"/>
+      <c r="A30" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
@@ -8353,15 +8540,8 @@
       <c r="I30" s="12"/>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="11"/>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
@@ -8371,13 +8551,13 @@
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
@@ -8387,8 +8567,15 @@
       <c r="I32" s="12"/>
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="10"/>
-      <c r="C33" s="11"/>
+      <c r="A33" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
@@ -8397,15 +8584,8 @@
       <c r="I33" s="12"/>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="11"/>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
@@ -8415,13 +8595,13 @@
     </row>
     <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
@@ -8432,13 +8612,13 @@
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
@@ -8448,8 +8628,15 @@
       <c r="I36" s="12"/>
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="13"/>
-      <c r="C37" s="11"/>
+      <c r="A37" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
@@ -8457,12 +8644,9 @@
       <c r="H37" s="12"/>
       <c r="I37" s="12"/>
     </row>
-    <row r="38" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="12"/>
+    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="13"/>
+      <c r="C38" s="11"/>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
@@ -8470,16 +8654,12 @@
       <c r="H38" s="12"/>
       <c r="I38" s="12"/>
     </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>70</v>
-      </c>
+    <row r="39" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" s="10"/>
+      <c r="C39" s="12"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
@@ -8487,15 +8667,15 @@
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
     </row>
-    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
@@ -8506,13 +8686,13 @@
     </row>
     <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
@@ -8523,13 +8703,13 @@
     </row>
     <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
@@ -8540,13 +8720,13 @@
     </row>
     <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
@@ -8556,8 +8736,15 @@
       <c r="I43" s="12"/>
     </row>
     <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B44" s="10"/>
-      <c r="C44" s="11"/>
+      <c r="A44" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
@@ -8565,10 +8752,7 @@
       <c r="H44" s="12"/>
       <c r="I44" s="12"/>
     </row>
-    <row r="45" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
-        <v>119</v>
-      </c>
+    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B45" s="10"/>
       <c r="C45" s="11"/>
       <c r="D45" s="12"/>
@@ -8578,16 +8762,12 @@
       <c r="H45" s="12"/>
       <c r="I45" s="12"/>
     </row>
-    <row r="46" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>70</v>
-      </c>
+    <row r="46" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="11"/>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
@@ -8595,15 +8775,15 @@
       <c r="H46" s="12"/>
       <c r="I46" s="12"/>
     </row>
-    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
@@ -8614,13 +8794,13 @@
     </row>
     <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
@@ -8631,13 +8811,13 @@
     </row>
     <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
@@ -8648,13 +8828,13 @@
     </row>
     <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="15" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
@@ -8665,13 +8845,13 @@
     </row>
     <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
@@ -8681,8 +8861,15 @@
       <c r="I51" s="12"/>
     </row>
     <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B52" s="13"/>
-      <c r="C52" s="12"/>
+      <c r="A52" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="D52" s="12"/>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
@@ -8690,14 +8877,9 @@
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
     </row>
-    <row r="53" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="17" t="s">
-        <v>130</v>
-      </c>
+    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B53" s="13"/>
-      <c r="C53" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="C53" s="12"/>
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
@@ -8705,15 +8887,13 @@
       <c r="H53" s="12"/>
       <c r="I53" s="12"/>
     </row>
-    <row r="54" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="B54" s="10" t="s">
-        <v>132</v>
-      </c>
+    <row r="54" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" s="13"/>
       <c r="C54" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
@@ -8722,15 +8902,15 @@
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
     </row>
-    <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
@@ -8741,13 +8921,13 @@
     </row>
     <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="15" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
@@ -8758,13 +8938,13 @@
     </row>
     <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="15" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
@@ -8775,13 +8955,13 @@
     </row>
     <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D58" s="12"/>
       <c r="E58" s="12"/>
@@ -8792,13 +8972,13 @@
     </row>
     <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
@@ -8808,8 +8988,15 @@
       <c r="I59" s="12"/>
     </row>
     <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B60" s="10"/>
-      <c r="C60" s="11"/>
+      <c r="A60" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="D60" s="12"/>
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
@@ -8817,10 +9004,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="12"/>
     </row>
-    <row r="61" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
-        <v>143</v>
-      </c>
+    <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B61" s="10"/>
       <c r="C61" s="11"/>
       <c r="D61" s="12"/>
@@ -8830,16 +9014,12 @@
       <c r="H61" s="12"/>
       <c r="I61" s="12"/>
     </row>
-    <row r="62" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B62" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>70</v>
-      </c>
+    <row r="62" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B62" s="10"/>
+      <c r="C62" s="11"/>
       <c r="D62" s="12"/>
       <c r="E62" s="12"/>
       <c r="F62" s="12"/>
@@ -8847,15 +9027,15 @@
       <c r="H62" s="12"/>
       <c r="I62" s="12"/>
     </row>
-    <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
@@ -8866,13 +9046,13 @@
     </row>
     <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D64" s="12"/>
       <c r="E64" s="12"/>
@@ -8883,13 +9063,13 @@
     </row>
     <row r="65" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D65" s="12"/>
       <c r="E65" s="12"/>
@@ -8900,13 +9080,13 @@
     </row>
     <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="15" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D66" s="12"/>
       <c r="E66" s="12"/>
@@ -8917,13 +9097,13 @@
     </row>
     <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D67" s="12"/>
       <c r="E67" s="12"/>
@@ -8934,13 +9114,13 @@
     </row>
     <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="15" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D68" s="12"/>
       <c r="E68" s="12"/>
@@ -8951,13 +9131,13 @@
     </row>
     <row r="69" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="15" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D69" s="12"/>
       <c r="E69" s="12"/>
@@ -8968,13 +9148,13 @@
     </row>
     <row r="70" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="15" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D70" s="12"/>
       <c r="E70" s="12"/>
@@ -8985,13 +9165,13 @@
     </row>
     <row r="71" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="15" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>84</v>
+        <v>155</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D71" s="12"/>
       <c r="E71" s="12"/>
@@ -9002,13 +9182,13 @@
     </row>
     <row r="72" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>164</v>
+        <v>78</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D72" s="12"/>
       <c r="E72" s="12"/>
@@ -9018,8 +9198,15 @@
       <c r="I72" s="12"/>
     </row>
     <row r="73" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B73" s="13"/>
-      <c r="C73" s="12"/>
+      <c r="A73" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
       <c r="F73" s="12"/>
@@ -9027,12 +9214,9 @@
       <c r="H73" s="12"/>
       <c r="I73" s="12"/>
     </row>
-    <row r="74" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="B74" s="10"/>
-      <c r="C74" s="11"/>
+    <row r="74" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B74" s="13"/>
+      <c r="C74" s="12"/>
       <c r="D74" s="12"/>
       <c r="E74" s="12"/>
       <c r="F74" s="12"/>
@@ -9040,16 +9224,12 @@
       <c r="H74" s="12"/>
       <c r="I74" s="12"/>
     </row>
-    <row r="75" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="B75" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>70</v>
-      </c>
+    <row r="75" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B75" s="10"/>
+      <c r="C75" s="11"/>
       <c r="D75" s="12"/>
       <c r="E75" s="12"/>
       <c r="F75" s="12"/>
@@ -9057,15 +9237,15 @@
       <c r="H75" s="12"/>
       <c r="I75" s="12"/>
     </row>
-    <row r="76" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A76" s="15" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D76" s="12"/>
       <c r="E76" s="12"/>
@@ -9076,13 +9256,13 @@
     </row>
     <row r="77" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="15" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D77" s="12"/>
       <c r="E77" s="12"/>
@@ -9093,13 +9273,13 @@
     </row>
     <row r="78" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D78" s="12"/>
       <c r="E78" s="12"/>
@@ -9110,13 +9290,13 @@
     </row>
     <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="15" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D79" s="12"/>
       <c r="E79" s="12"/>
@@ -9127,13 +9307,13 @@
     </row>
     <row r="80" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A80" s="15" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D80" s="12"/>
       <c r="E80" s="12"/>
@@ -9144,13 +9324,13 @@
     </row>
     <row r="81" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="15" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D81" s="12"/>
       <c r="E81" s="12"/>
@@ -9161,13 +9341,13 @@
     </row>
     <row r="82" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="15" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D82" s="12"/>
       <c r="E82" s="12"/>
@@ -9178,13 +9358,13 @@
     </row>
     <row r="83" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A83" s="15" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="12"/>
@@ -9195,13 +9375,13 @@
     </row>
     <row r="84" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="15" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D84" s="12"/>
       <c r="E84" s="12"/>
@@ -9212,13 +9392,13 @@
     </row>
     <row r="85" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A85" s="15" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D85" s="12"/>
       <c r="E85" s="12"/>
@@ -9229,13 +9409,13 @@
     </row>
     <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A86" s="15" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D86" s="12"/>
       <c r="E86" s="12"/>
@@ -9245,8 +9425,15 @@
       <c r="I86" s="12"/>
     </row>
     <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B87" s="13"/>
-      <c r="C87" s="12"/>
+      <c r="A87" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="D87" s="12"/>
       <c r="E87" s="12"/>
       <c r="F87" s="12"/>
@@ -9254,10 +9441,7 @@
       <c r="H87" s="12"/>
       <c r="I87" s="12"/>
     </row>
-    <row r="88" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="17" t="s">
-        <v>190</v>
-      </c>
+    <row r="88" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B88" s="13"/>
       <c r="C88" s="12"/>
       <c r="D88" s="12"/>
@@ -9267,34 +9451,28 @@
       <c r="H88" s="12"/>
       <c r="I88" s="12"/>
     </row>
-    <row r="89" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="B89" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="C89" s="11" t="s">
-        <v>70</v>
-      </c>
+    <row r="89" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B89" s="13"/>
+      <c r="C89" s="12"/>
       <c r="D89" s="12"/>
       <c r="E89" s="12"/>
       <c r="F89" s="12"/>
-      <c r="G89" s="11" t="s">
-        <v>11</v>
-      </c>
+      <c r="G89" s="12"/>
       <c r="H89" s="12"/>
       <c r="I89" s="12"/>
     </row>
-    <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A90" s="15" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D90" s="12"/>
       <c r="E90" s="12"/>
@@ -9307,13 +9485,13 @@
     </row>
     <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A91" s="15" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D91" s="12"/>
       <c r="E91" s="12"/>
@@ -9326,13 +9504,13 @@
     </row>
     <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A92" s="15" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D92" s="12"/>
       <c r="E92" s="12"/>
@@ -9345,13 +9523,13 @@
     </row>
     <row r="93" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A93" s="15" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D93" s="12"/>
       <c r="E93" s="12"/>
@@ -9364,13 +9542,13 @@
     </row>
     <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A94" s="15" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D94" s="12"/>
       <c r="E94" s="12"/>
@@ -9383,13 +9561,13 @@
     </row>
     <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A95" s="15" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D95" s="12"/>
       <c r="E95" s="12"/>
@@ -9402,13 +9580,13 @@
     </row>
     <row r="96" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="15" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D96" s="12"/>
       <c r="E96" s="12"/>
@@ -9420,19 +9598,25 @@
       <c r="I96" s="12"/>
     </row>
     <row r="97" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B97" s="13"/>
-      <c r="C97" s="12"/>
+      <c r="A97" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="B97" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="D97" s="12"/>
       <c r="E97" s="12"/>
       <c r="F97" s="12"/>
-      <c r="G97" s="12"/>
+      <c r="G97" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="H97" s="12"/>
       <c r="I97" s="12"/>
     </row>
-    <row r="98" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="17" t="s">
-        <v>207</v>
-      </c>
+    <row r="98" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B98" s="13"/>
       <c r="C98" s="12"/>
       <c r="D98" s="12"/>
@@ -9442,16 +9626,12 @@
       <c r="H98" s="12"/>
       <c r="I98" s="12"/>
     </row>
-    <row r="99" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="B99" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="C99" s="11" t="s">
-        <v>70</v>
-      </c>
+    <row r="99" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="B99" s="13"/>
+      <c r="C99" s="12"/>
       <c r="D99" s="12"/>
       <c r="E99" s="12"/>
       <c r="F99" s="12"/>
@@ -9459,15 +9639,15 @@
       <c r="H99" s="12"/>
       <c r="I99" s="12"/>
     </row>
-    <row r="100" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A100" s="15" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D100" s="12"/>
       <c r="E100" s="12"/>
@@ -9478,13 +9658,13 @@
     </row>
     <row r="101" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A101" s="15" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D101" s="12"/>
       <c r="E101" s="12"/>
@@ -9495,13 +9675,13 @@
     </row>
     <row r="102" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A102" s="15" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D102" s="12"/>
       <c r="E102" s="12"/>
@@ -9512,13 +9692,13 @@
     </row>
     <row r="103" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="15" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B103" s="10" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D103" s="12"/>
       <c r="E103" s="12"/>
@@ -9529,13 +9709,13 @@
     </row>
     <row r="104" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A104" s="15" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D104" s="12"/>
       <c r="E104" s="12"/>
@@ -9546,13 +9726,13 @@
     </row>
     <row r="105" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A105" s="15" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D105" s="12"/>
       <c r="E105" s="12"/>
@@ -9563,13 +9743,13 @@
     </row>
     <row r="106" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A106" s="15" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D106" s="12"/>
       <c r="E106" s="12"/>
@@ -9580,13 +9760,13 @@
     </row>
     <row r="107" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A107" s="15" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B107" s="10" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D107" s="12"/>
       <c r="E107" s="12"/>
@@ -9597,13 +9777,13 @@
     </row>
     <row r="108" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="15" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D108" s="12"/>
       <c r="E108" s="12"/>
@@ -9614,13 +9794,13 @@
     </row>
     <row r="109" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A109" s="15" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D109" s="12"/>
       <c r="E109" s="12"/>
@@ -9631,13 +9811,13 @@
     </row>
     <row r="110" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A110" s="15" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D110" s="12"/>
       <c r="E110" s="12"/>
@@ -9648,13 +9828,13 @@
     </row>
     <row r="111" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A111" s="15" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B111" s="10" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D111" s="12"/>
       <c r="E111" s="12"/>
@@ -9664,8 +9844,15 @@
       <c r="I111" s="12"/>
     </row>
     <row r="112" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B112" s="11"/>
-      <c r="C112" s="11"/>
+      <c r="A112" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B112" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C112" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="D112" s="12"/>
       <c r="E112" s="12"/>
       <c r="F112" s="12"/>
@@ -9724,8 +9911,8 @@
       <c r="I117" s="12"/>
     </row>
     <row r="118" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B118" s="12"/>
-      <c r="C118" s="12"/>
+      <c r="B118" s="11"/>
+      <c r="C118" s="11"/>
       <c r="D118" s="12"/>
       <c r="E118" s="12"/>
       <c r="F118" s="12"/>
@@ -9744,8 +9931,8 @@
       <c r="I119" s="12"/>
     </row>
     <row r="120" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B120" s="11"/>
-      <c r="C120" s="11"/>
+      <c r="B120" s="12"/>
+      <c r="C120" s="12"/>
       <c r="D120" s="12"/>
       <c r="E120" s="12"/>
       <c r="F120" s="12"/>
@@ -9754,8 +9941,8 @@
       <c r="I120" s="12"/>
     </row>
     <row r="121" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B121" s="12"/>
-      <c r="C121" s="12"/>
+      <c r="B121" s="11"/>
+      <c r="C121" s="11"/>
       <c r="D121" s="12"/>
       <c r="E121" s="12"/>
       <c r="F121" s="12"/>
@@ -9774,8 +9961,8 @@
       <c r="I122" s="12"/>
     </row>
     <row r="123" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B123" s="11"/>
-      <c r="C123" s="11"/>
+      <c r="B123" s="12"/>
+      <c r="C123" s="12"/>
       <c r="D123" s="12"/>
       <c r="E123" s="12"/>
       <c r="F123" s="12"/>
@@ -9794,7 +9981,7 @@
       <c r="I124" s="12"/>
     </row>
     <row r="125" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B125" s="12"/>
+      <c r="B125" s="11"/>
       <c r="C125" s="11"/>
       <c r="D125" s="12"/>
       <c r="E125" s="12"/>
@@ -9835,7 +10022,7 @@
     </row>
     <row r="129" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B129" s="12"/>
-      <c r="C129" s="12"/>
+      <c r="C129" s="11"/>
       <c r="D129" s="12"/>
       <c r="E129" s="12"/>
       <c r="F129" s="12"/>
@@ -19302,6 +19489,16 @@
       <c r="G1075" s="12"/>
       <c r="H1075" s="12"/>
       <c r="I1075" s="12"/>
+    </row>
+    <row r="1076" spans="2:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B1076" s="12"/>
+      <c r="C1076" s="12"/>
+      <c r="D1076" s="12"/>
+      <c r="E1076" s="12"/>
+      <c r="F1076" s="12"/>
+      <c r="G1076" s="12"/>
+      <c r="H1076" s="12"/>
+      <c r="I1076" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -19341,21 +19538,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="1"/>
@@ -19381,7 +19578,7 @@
       <c r="AD1" s="1"/>
     </row>
     <row r="2" spans="1:30" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
+      <c r="A2" s="25"/>
       <c r="B2" s="19" t="s">
         <v>4</v>
       </c>
@@ -19403,7 +19600,7 @@
       <c r="H2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="22"/>
+      <c r="I2" s="25"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -19428,7 +19625,7 @@
     </row>
     <row r="3" spans="1:30" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -19462,7 +19659,7 @@
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
@@ -19472,7 +19669,7 @@
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>11</v>
@@ -19482,7 +19679,7 @@
     </row>
     <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
@@ -19493,7 +19690,7 @@
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
@@ -19503,7 +19700,7 @@
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
@@ -19519,7 +19716,7 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -19528,7 +19725,7 @@
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -19538,7 +19735,7 @@
     </row>
     <row r="12" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -19548,7 +19745,7 @@
     </row>
     <row r="13" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -19558,7 +19755,7 @@
     </row>
     <row r="14" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -19568,7 +19765,7 @@
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -25359,132 +25556,132 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="26" t="s">
-        <v>329</v>
+      <c r="A28" s="24" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="25" t="s">
-        <v>257</v>
+      <c r="A29" s="23" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="25" t="s">
-        <v>258</v>
+      <c r="A30" s="23" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="25" t="s">
-        <v>259</v>
+      <c r="A31" s="23" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="25" t="s">
-        <v>260</v>
+      <c r="A32" s="23" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -25511,112 +25708,112 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25627,12 +25824,12 @@
     </row>
     <row r="29" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25640,32 +25837,32 @@
     </row>
     <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15" x14ac:dyDescent="0.2">
@@ -25673,22 +25870,22 @@
     </row>
     <row r="39" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="15" x14ac:dyDescent="0.2">
@@ -25696,17 +25893,17 @@
     </row>
     <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="15" x14ac:dyDescent="0.2">
@@ -25714,67 +25911,67 @@
     </row>
     <row r="48" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="15" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="15" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="15" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="15" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="15" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15" x14ac:dyDescent="0.2">
@@ -25782,47 +25979,47 @@
     </row>
     <row r="62" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="26" t="s">
-        <v>329</v>
+      <c r="A70" s="24" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="15" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="15" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>